<commit_message>
Agregando crud de productos
</commit_message>
<xml_diff>
--- a/storage/app/utils/Tables.xlsx
+++ b/storage/app/utils/Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crm.atalaya\storage\app\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29B5F0F-8B9B-4A18-BF7F-0A4BD3128EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C709214C-33C3-4098-8F20-925691003319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>9c27e649-574a-47eb-82af-851c5d425434</t>
+  </si>
+  <si>
+    <t>1783c832-8dfb-4d30-810c-bc88345507bf</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Tabla de productos</t>
   </si>
 </sst>
 </file>
@@ -128,9 +137,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +424,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +539,21 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F11" s="1"/>

</xml_diff>